<commit_message>
adding additional user attributes Name Pronounciation Dietary Preference Photo Release Complete IEIN Admin notes to Excel User template
</commit_message>
<xml_diff>
--- a/bcse_site/bcse_app/static/xls/UserTemplate.xlsx
+++ b/bcse_site/bcse_app/static/xls/UserTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snp146/bcse/bcse_site/bcse_app/static/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D24603-53E5-3C41-AE10-7CA92026C6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23C5FEE-175A-2A46-A6C1-9F2EE89D172B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31460" yWindow="640" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B5201E93-1EAE-7D4F-AF55-CCC0B5A3E04D}"/>
+    <workbookView xWindow="38380" yWindow="1000" windowWidth="28040" windowHeight="17440" xr2:uid="{B5201E93-1EAE-7D4F-AF55-CCC0B5A3E04D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>BCSE Admin</t>
   </si>
@@ -160,6 +160,24 @@
   </si>
   <si>
     <t>K-12 Teacher or Administrator</t>
+  </si>
+  <si>
+    <t>Name Pronounciation</t>
+  </si>
+  <si>
+    <t>Dietary Preference</t>
+  </si>
+  <si>
+    <t>Photo Release Complete?</t>
+  </si>
+  <si>
+    <t>IEIN</t>
+  </si>
+  <si>
+    <t>Admin Notes</t>
+  </si>
+  <si>
+    <t>Workplace ID</t>
   </si>
 </sst>
 </file>
@@ -230,9 +248,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -270,7 +288,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -376,7 +394,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -518,7 +536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -526,11 +544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE7D386-0738-944D-BD9A-00E3C44559D0}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,9 +558,14 @@
     <col min="4" max="4" width="25.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -564,8 +587,31 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{95C68B3A-8B29-A841-BDCB-78C5259BC022}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -586,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B7BDD3-2C5D-8E45-8C3D-CA8D30BFB067}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>